<commit_message>
chartfx files and action update
</commit_message>
<xml_diff>
--- a/action list.xlsx
+++ b/action list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
   <si>
     <t>ITEM</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Remove all cmdlib, save/load cmds</t>
+  </si>
+  <si>
+    <t>Parametric Studies</t>
   </si>
 </sst>
 </file>
@@ -631,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD53"/>
+  <dimension ref="A1:XFD54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="D50" sqref="A50:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,53 +1364,65 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C50" s="3"/>
       <c r="D50" s="4">
-        <v>41818</v>
+        <v>42160</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D51" s="4">
-        <v>41796</v>
+        <v>41818</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
       </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D52" s="4">
         <v>41796</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="4">
+        <v>41796</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="4">
         <v>41796</v>
       </c>
     </row>

</xml_diff>